<commit_message>
Updated resource list with sugarcane
</commit_message>
<xml_diff>
--- a/Story/Resource List (updated).xlsx
+++ b/Story/Resource List (updated).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Exilium\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Exilium\Documents\Senior Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5201665D-E04F-42F6-9E12-17645E6B4C57}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37446ACD-2618-408F-B747-41A24EABE46D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="202">
   <si>
     <t>Name of Resource</t>
   </si>
@@ -611,6 +611,21 @@
   </si>
   <si>
     <t>Crop, Fiber, Ingredient</t>
+  </si>
+  <si>
+    <t>SUGARCANE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Known as "reeds that produce honey without bees. Sugarcane is a very tall plant that can grow up to 20 feet tall. The tall stalks are rich in sugar and can be processed in various ways or eaten raw. </t>
+  </si>
+  <si>
+    <t>3 coins per stalk</t>
+  </si>
+  <si>
+    <t>Food, Crop, Plant, Ingredient</t>
+  </si>
+  <si>
+    <t>A long reed filled with raw sugar.</t>
   </si>
 </sst>
 </file>
@@ -1067,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1000"/>
+  <dimension ref="A1:K1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1703,201 +1718,217 @@
         <v>136</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D37" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D38" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D39" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D40" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D41" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E41" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D42" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D43" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D44" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D45" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E45" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D46" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E46" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D47" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E47" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-    </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+    </row>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2850,6 +2881,7 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added resources, added Capital description, grammar checks
</commit_message>
<xml_diff>
--- a/Story/Resource List (updated).xlsx
+++ b/Story/Resource List (updated).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Exilium\Documents\Senior Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37446ACD-2618-408F-B747-41A24EABE46D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC7BCF0-BD6F-411E-BC39-E2B9D89AF2B5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="204">
   <si>
     <t>Name of Resource</t>
   </si>
@@ -163,9 +163,6 @@
     <t xml:space="preserve">A soft fiber that grows from cotton plants. The fiber is used to create yarn or threads and woven into textiles and clothing. </t>
   </si>
   <si>
-    <t>30 chips per bundle</t>
-  </si>
-  <si>
     <t>A bundle of cotton. Not as soft as you thought it would be… Needs to be processed somehow.</t>
   </si>
   <si>
@@ -253,9 +250,6 @@
     <t>GOLD INGOT</t>
   </si>
   <si>
-    <t>A bar of solid gold and mostly hoarded by the wealthy. Used to make objects of seeming importance such as crowns.</t>
-  </si>
-  <si>
     <t>A bar of solid gold! Quite heavy. Should you really try to make something out of this?</t>
   </si>
   <si>
@@ -316,9 +310,6 @@
     <t>LINEN</t>
   </si>
   <si>
-    <t xml:space="preserve">Fabric spun from flax. Can be spun into a thick or thin fabric. Softer and more comfortable than wool and as such, preferred for undergarments or summer wear. </t>
-  </si>
-  <si>
     <t>1.5 royals per roll</t>
   </si>
   <si>
@@ -361,9 +352,6 @@
     <t>RUBY</t>
   </si>
   <si>
-    <t xml:space="preserve">An extremely precious stone. A regal red stone, equally prized as the sapphire. Associated with good health and youth. Owning a ruby signified great wealth and social status. </t>
-  </si>
-  <si>
     <t>5 royals per stone</t>
   </si>
   <si>
@@ -626,6 +614,24 @@
   </si>
   <si>
     <t>A long reed filled with raw sugar.</t>
+  </si>
+  <si>
+    <t>A bar of solid gold and mostly hoarded by the wealthy. Used to make objects of seeming importance, such as crowns.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An extremely precious stone. A regal red stone, equally prized as the sapphire. Associated with good health and youth. Owning a ruby signifies great wealth and social status. </t>
+  </si>
+  <si>
+    <t>COTTON PLANT</t>
+  </si>
+  <si>
+    <t>Fabric spun from flax. Can be spun into a thick or thin fabric. Softer and more comfortable than wool and as such, preferred for undergarments or summer wear. Seen as an alternative to cotton.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A roll of cotton. You can probably make some clothes out of this. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fabric spun from cotton fiber. Very soft, comfortable and perfect for undergarments. Seen as an alternative to linen. </t>
   </si>
 </sst>
 </file>
@@ -643,17 +649,20 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1082,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1001"/>
+  <dimension ref="A1:K1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1110,7 +1119,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -1127,7 +1136,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>7</v>
@@ -1148,7 +1157,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
@@ -1169,7 +1178,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>17</v>
@@ -1190,7 +1199,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>22</v>
@@ -1211,7 +1220,7 @@
         <v>26</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>27</v>
@@ -1232,7 +1241,7 @@
         <v>31</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>32</v>
@@ -1253,7 +1262,7 @@
         <v>36</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>37</v>
@@ -1270,7 +1279,7 @@
         <v>40</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>41</v>
@@ -1287,664 +1296,680 @@
         <v>40</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="E11" s="3" t="s">
+    </row>
+    <row r="13" spans="1:11" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D13" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="E12" s="3" t="s">
+    </row>
+    <row r="14" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D14" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="E13" s="3" t="s">
+    </row>
+    <row r="15" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D15" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="E14" s="3" t="s">
+    </row>
+    <row r="16" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D16" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="E15" s="3" t="s">
+    </row>
+    <row r="17" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D17" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D19" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>117</v>
+        <v>199</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>114</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E31" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="34" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B34" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>135</v>
+        <v>40</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    </row>
+    <row r="38" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D37" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="D39" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="40" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="E38" s="3" t="s">
+      <c r="D40" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="41" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D39" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="E39" s="3" t="s">
+      <c r="D41" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="42" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C42" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D40" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="E40" s="3" t="s">
+    </row>
+    <row r="43" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="B43" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="C43" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="E41" s="3" t="s">
+    </row>
+    <row r="44" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="B44" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="C44" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="E42" s="3" t="s">
+    </row>
+    <row r="45" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="B45" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="E43" s="3" t="s">
+      <c r="D45" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="46" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C46" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="E44" s="3" t="s">
+    </row>
+    <row r="47" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="B47" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="C47" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="E45" s="3" t="s">
+    </row>
+    <row r="48" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="B48" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="E46" s="3" t="s">
+      <c r="D48" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-    </row>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2882,6 +2907,7 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>